<commit_message>
updated data_structure documentation and renamed series_cleaner to series_correction
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Documents\FVA\Gartiser_Valentin\ConFluxPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2A70E1-3E98-489E-B5C9-280359AA9864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEFFF67-778F-4A93-A038-1719732E4C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{07E2472D-221B-4994-9FCF-2F14B0061AAA}"/>
+    <workbookView xWindow="4100" yWindow="4100" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{07E2472D-221B-4994-9FCF-2F14B0061AAA}"/>
   </bookViews>
   <sheets>
     <sheet name="gasdata" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
   <si>
     <t>Plot</t>
   </si>
@@ -85,9 +85,6 @@
     <t>the actual depth of the sampler</t>
   </si>
   <si>
-    <t>humheight</t>
-  </si>
-  <si>
     <t>atmosphere/soil interface depth</t>
   </si>
   <si>
@@ -125,6 +122,195 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>variable name</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>n.a.</t>
+  </si>
+  <si>
+    <t>L/L</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>hPa</t>
+  </si>
+  <si>
+    <t>m^2/s</t>
+  </si>
+  <si>
+    <t>complete_soilphys</t>
+  </si>
+  <si>
+    <t>rho_air</t>
+  </si>
+  <si>
+    <t>mol/m^3</t>
+  </si>
+  <si>
+    <t>original data</t>
+  </si>
+  <si>
+    <t>discretize_depth(); join_soilphys(); complete_soilphys(); calculate_flux()</t>
+  </si>
+  <si>
+    <t>complete_soilphys()</t>
+  </si>
+  <si>
+    <t>calculate_flux()</t>
+  </si>
+  <si>
+    <t>the mean depth of the layer</t>
+  </si>
+  <si>
+    <t>upper bound of the layer</t>
+  </si>
+  <si>
+    <t>lower bound of the layer</t>
+  </si>
+  <si>
+    <t>the gas for which the diffusion coefficients relate to. Is created in complete_soilphys()</t>
+  </si>
+  <si>
+    <t>the Total Pore Space as volumetric fraction relative to total volume</t>
+  </si>
+  <si>
+    <t>Soil Water Content as volumetric fraction relative to the total volume</t>
+  </si>
+  <si>
+    <t>mean soil temperature of the layer</t>
+  </si>
+  <si>
+    <t>mean pressure of the layer</t>
+  </si>
+  <si>
+    <t>Ratio of apparent to effective diffusion coefficient</t>
+  </si>
+  <si>
+    <t>effective diffusion coefficient of a gas</t>
+  </si>
+  <si>
+    <t>apparent diffusion coefficient of a gas</t>
+  </si>
+  <si>
+    <t>mean molar density of the air in the layer</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>upper-lower</t>
+  </si>
+  <si>
+    <t>height of the layer</t>
+  </si>
+  <si>
+    <t>V_pores /V_total</t>
+  </si>
+  <si>
+    <t>V_water/V_total</t>
+  </si>
+  <si>
+    <t>V_air/V_total = TPS-SWC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Filled Pore Space as volumetric fraction relative to total volume </t>
+  </si>
+  <si>
+    <t>f(AFPS)</t>
+  </si>
+  <si>
+    <t>a*Temp^(b*p)</t>
+  </si>
+  <si>
+    <t>DSD0*D0</t>
+  </si>
+  <si>
+    <t>p/(RT)</t>
+  </si>
+  <si>
+    <t>ppmv</t>
+  </si>
+  <si>
+    <t>topheight</t>
+  </si>
+  <si>
+    <t>missing_gas</t>
+  </si>
+  <si>
+    <t>corr_fac</t>
+  </si>
+  <si>
+    <t>depth_cat</t>
+  </si>
+  <si>
+    <t>bal</t>
+  </si>
+  <si>
+    <t>bal_flag</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>p_gas/p</t>
+  </si>
+  <si>
+    <t>grouping different gas wells into categories, even though their specific depth might differ (e.g. "Humus","-5cm")</t>
+  </si>
+  <si>
+    <t>sum(NRESULT_ppm(gases))</t>
+  </si>
+  <si>
+    <t>which gases were missing in the balance correction</t>
+  </si>
+  <si>
+    <t>the sum of the concentration of all gases of a sample. Should be 1 in an ideal measurement</t>
+  </si>
+  <si>
+    <t>True if the sample was not corrected in the balance approach</t>
+  </si>
+  <si>
+    <t>the correction factor in the offset approach</t>
+  </si>
+  <si>
+    <t>balance_correction()</t>
+  </si>
+  <si>
+    <t>offset_correction</t>
+  </si>
+  <si>
+    <t>balance_correction();</t>
+  </si>
+  <si>
+    <t>series_correction(); offset_correction(); calculate_flux()</t>
+  </si>
+  <si>
+    <t>series_correction(); offset_correction(); balance_correction(); calculate_flux()</t>
+  </si>
+  <si>
+    <t>series_correction()</t>
   </si>
 </sst>
 </file>
@@ -164,10 +350,30 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -176,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -185,6 +391,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,57 +723,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28948E16-6373-4601-A228-026AD168681D}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" customWidth="1"/>
+    <col min="7" max="7" width="24.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="15.90625" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="25.6328125" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -559,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>6</v>
@@ -567,31 +816,225 @@
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -602,86 +1045,386 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5DC2B6-D665-423D-8F8F-385C795712DF}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="5" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="24.26953125" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="15" max="15" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="11" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="P7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -700,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>

</xml_diff>